<commit_message>
refined dashboards after week 10 presentation
Includes word-cloud in dashboard, and the necessary files to generate it (word_file excel and word-separator jupyter nb)
</commit_message>
<xml_diff>
--- a/Krissy_Tableau/feedback_data_for_training.xlsx
+++ b/Krissy_Tableau/feedback_data_for_training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krissy\Dropbox\W210-Capstone\_Project Materials\Krissy_Tableau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79193AF5-6702-40C3-BA4D-CD5546DD3865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AB4D74-7815-4E43-A37F-54CDFA3AF671}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="930" windowWidth="18975" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="2040" windowWidth="19440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="227">
   <si>
     <t>source</t>
   </si>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t>the problem sets have only been doable because of the study group we put together. if we weren't able to work together on these, i don't know if i'd be able to keep up.</t>
-  </si>
-  <si>
-    <t>DUPLICATE?</t>
   </si>
   <si>
     <t>there is only one instructor who is semi-responsive on Slack. So, students are trying to figure out the issues on their own through the week.</t>
@@ -1104,8 +1101,8 @@
   </sheetPr>
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H159" sqref="H159:H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1122,13 +1119,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1146,15 +1143,15 @@
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:B65" ca="1" si="0">CHOOSE(RANDBETWEEN(1,10), 200,201,203,207,209,210,241,231,266, "W266")</f>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">RANDBETWEEN(DATE(2018,1,1),DATE(2019,3,1))</f>
-        <v>43297</v>
+        <v>43392</v>
       </c>
       <c r="D2" s="7">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1172,15 +1169,15 @@
       </c>
       <c r="B3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="6">
         <f t="shared" ref="C3:C66" ca="1" si="1">RANDBETWEEN(DATE(2018,1,1),DATE(2019,3,1))</f>
-        <v>43278</v>
+        <v>43167</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:D66" ca="1" si="2">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>20</v>
@@ -1198,15 +1195,15 @@
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43497</v>
+        <v>43116</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>22</v>
@@ -1224,15 +1221,15 @@
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43126</v>
+        <v>43488</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -1250,11 +1247,11 @@
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>266</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43449</v>
+        <v>43286</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1273,15 +1270,15 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43354</v>
+        <v>43444</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>31</v>
@@ -1303,11 +1300,11 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43438</v>
+        <v>43449</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>37</v>
@@ -1325,15 +1322,15 @@
       </c>
       <c r="B9" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43343</v>
+        <v>43136</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>41</v>
@@ -1355,11 +1352,11 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43387</v>
+        <v>43410</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>43</v>
@@ -1377,15 +1374,15 @@
       </c>
       <c r="B11" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43184</v>
+        <v>43335</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>44</v>
@@ -1403,15 +1400,15 @@
       </c>
       <c r="B12" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43496</v>
+        <v>43229</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>45</v>
@@ -1433,11 +1430,11 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43488</v>
+        <v>43134</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>46</v>
@@ -1455,15 +1452,15 @@
       </c>
       <c r="B14" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43199</v>
+        <v>43356</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>47</v>
@@ -1481,15 +1478,15 @@
       </c>
       <c r="B15" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43197</v>
+        <v>43450</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>48</v>
@@ -1511,11 +1508,11 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43134</v>
+        <v>43243</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>49</v>
@@ -1531,13 +1528,13 @@
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="str">
+      <c r="B17" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>203</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43388</v>
+        <v>43152</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1559,11 +1556,11 @@
       </c>
       <c r="B18" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43516</v>
+        <v>43153</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1583,17 +1580,17 @@
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>W266</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43354</v>
+        <v>43427</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>52</v>
@@ -1609,17 +1606,17 @@
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="9" t="str">
+      <c r="B20" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>209</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43162</v>
+        <v>43155</v>
       </c>
       <c r="D20" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>53</v>
@@ -1641,11 +1638,11 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43404</v>
+        <v>43220</v>
       </c>
       <c r="D21" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>53</v>
@@ -1661,17 +1658,17 @@
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>W266</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43490</v>
+        <v>43283</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>54</v>
@@ -1689,11 +1686,11 @@
       </c>
       <c r="B23" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43373</v>
+        <v>43395</v>
       </c>
       <c r="D23" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1715,15 +1712,15 @@
       </c>
       <c r="B24" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43361</v>
+        <v>43400</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>56</v>
@@ -1739,17 +1736,17 @@
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>W266</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43163</v>
+        <v>43416</v>
       </c>
       <c r="D25" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>57</v>
@@ -1765,17 +1762,17 @@
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="9" t="str">
+      <c r="B26" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>209</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43176</v>
+        <v>43417</v>
       </c>
       <c r="D26" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>58</v>
@@ -1797,7 +1794,7 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43470</v>
+        <v>43249</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1819,15 +1816,15 @@
       </c>
       <c r="B28" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43356</v>
+        <v>43473</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>60</v>
@@ -1837,13 +1834,13 @@
       <c r="A29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="9" t="str">
+      <c r="B29" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>200</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43295</v>
+        <v>43518</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -1865,15 +1862,15 @@
       </c>
       <c r="B30" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43509</v>
+        <v>43278</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>62</v>
@@ -1891,15 +1888,15 @@
       </c>
       <c r="B31" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43277</v>
+        <v>43362</v>
       </c>
       <c r="D31" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>63</v>
@@ -1915,17 +1912,17 @@
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43483</v>
+        <v>43160</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>64</v>
@@ -1943,15 +1940,15 @@
       </c>
       <c r="B33" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43263</v>
+        <v>43160</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>65</v>
@@ -1969,15 +1966,15 @@
       </c>
       <c r="B34" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C34" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43321</v>
+        <v>43102</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>66</v>
@@ -1995,11 +1992,11 @@
       </c>
       <c r="B35" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>203</v>
       </c>
       <c r="C35" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43236</v>
+        <v>43334</v>
       </c>
       <c r="D35" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2021,15 +2018,15 @@
       </c>
       <c r="B36" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="C36" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43176</v>
+        <v>43175</v>
       </c>
       <c r="D36" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>69</v>
@@ -2047,15 +2044,15 @@
       </c>
       <c r="B37" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="C37" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43133</v>
+        <v>43192</v>
       </c>
       <c r="D37" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>69</v>
@@ -2073,15 +2070,15 @@
       </c>
       <c r="B38" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43176</v>
+        <v>43269</v>
       </c>
       <c r="D38" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>70</v>
@@ -2099,15 +2096,15 @@
       </c>
       <c r="B39" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43222</v>
+        <v>43490</v>
       </c>
       <c r="D39" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>71</v>
@@ -2125,11 +2122,11 @@
       </c>
       <c r="B40" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C40" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43273</v>
+        <v>43301</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2149,13 +2146,13 @@
       <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="9" t="str">
+      <c r="B41" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>210</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43484</v>
+        <v>43503</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2177,15 +2174,15 @@
       </c>
       <c r="B42" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43401</v>
+        <v>43235</v>
       </c>
       <c r="D42" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>73</v>
@@ -2203,15 +2200,15 @@
       </c>
       <c r="B43" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43297</v>
+        <v>43397</v>
       </c>
       <c r="D43" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>74</v>
@@ -2229,15 +2226,15 @@
       </c>
       <c r="B44" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C44" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43293</v>
+        <v>43478</v>
       </c>
       <c r="D44" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>75</v>
@@ -2253,13 +2250,13 @@
       <c r="A45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>W266</v>
       </c>
       <c r="C45" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43285</v>
+        <v>43384</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2279,13 +2276,13 @@
       <c r="A46" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="9" t="str">
+      <c r="B46" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>200</v>
       </c>
       <c r="C46" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43114</v>
+        <v>43417</v>
       </c>
       <c r="D46" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2305,13 +2302,13 @@
       <c r="A47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>W266</v>
       </c>
       <c r="C47" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43397</v>
+        <v>43292</v>
       </c>
       <c r="D47" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2331,17 +2328,17 @@
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="9" t="str">
+      <c r="B48" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>210</v>
       </c>
       <c r="C48" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43312</v>
+        <v>43241</v>
       </c>
       <c r="D48" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>78</v>
@@ -2354,17 +2351,17 @@
       <c r="A49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="9" t="str">
+      <c r="B49" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>200</v>
       </c>
       <c r="C49" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43167</v>
+        <v>43442</v>
       </c>
       <c r="D49" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>79</v>
@@ -2379,11 +2376,11 @@
       </c>
       <c r="B50" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C50" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43131</v>
+        <v>43316</v>
       </c>
       <c r="D50" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2405,15 +2402,15 @@
       </c>
       <c r="B51" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C51" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43105</v>
+        <v>43522</v>
       </c>
       <c r="D51" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>81</v>
@@ -2431,11 +2428,11 @@
       </c>
       <c r="B52" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="C52" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43423</v>
+        <v>43492</v>
       </c>
       <c r="D52" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2457,15 +2454,15 @@
       </c>
       <c r="B53" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C53" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43506</v>
+        <v>43227</v>
       </c>
       <c r="D53" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>84</v>
@@ -2481,13 +2478,13 @@
       <c r="A54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="9" t="str">
+      <c r="B54" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>W266</v>
+        <v>210</v>
       </c>
       <c r="C54" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43496</v>
+        <v>43374</v>
       </c>
       <c r="D54" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2509,11 +2506,11 @@
       </c>
       <c r="B55" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C55" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43207</v>
+        <v>43174</v>
       </c>
       <c r="D55" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2535,15 +2532,15 @@
       </c>
       <c r="B56" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C56" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43136</v>
+        <v>43107</v>
       </c>
       <c r="D56" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>87</v>
@@ -2559,17 +2556,17 @@
       <c r="A57" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C57" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43428</v>
+        <v>43155</v>
       </c>
       <c r="D57" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>88</v>
@@ -2587,11 +2584,11 @@
       </c>
       <c r="B58" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>266</v>
       </c>
       <c r="C58" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43116</v>
+        <v>43126</v>
       </c>
       <c r="D58" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2613,15 +2610,15 @@
       </c>
       <c r="B59" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C59" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43506</v>
+        <v>43500</v>
       </c>
       <c r="D59" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>90</v>
@@ -2639,11 +2636,11 @@
       </c>
       <c r="B60" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="C60" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43139</v>
+        <v>43250</v>
       </c>
       <c r="D60" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2665,11 +2662,11 @@
       </c>
       <c r="B61" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C61" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43250</v>
+        <v>43150</v>
       </c>
       <c r="D61" s="7">
         <f t="shared" ca="1" si="2"/>
@@ -2691,15 +2688,15 @@
       </c>
       <c r="B62" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="C62" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43134</v>
+        <v>43196</v>
       </c>
       <c r="D62" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>93</v>
@@ -2717,15 +2714,15 @@
       </c>
       <c r="B63" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C63" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43124</v>
+        <v>43244</v>
       </c>
       <c r="D63" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>94</v>
@@ -2741,17 +2738,17 @@
       <c r="A64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>W266</v>
       </c>
       <c r="C64" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43171</v>
+        <v>43233</v>
       </c>
       <c r="D64" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>95</v>
@@ -2769,15 +2766,15 @@
       </c>
       <c r="B65" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C65" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43383</v>
+        <v>43396</v>
       </c>
       <c r="D65" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>96</v>
@@ -2795,15 +2792,15 @@
       </c>
       <c r="B66" s="9">
         <f t="shared" ref="B66:B129" ca="1" si="3">CHOOSE(RANDBETWEEN(1,10), 200,201,203,207,209,210,241,231,266, "W266")</f>
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="C66" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43274</v>
+        <v>43248</v>
       </c>
       <c r="D66" s="7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>97</v>
@@ -2818,15 +2815,15 @@
       </c>
       <c r="B67" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>266</v>
       </c>
       <c r="C67" s="6">
         <f t="shared" ref="C67:C130" ca="1" si="4">RANDBETWEEN(DATE(2018,1,1),DATE(2019,3,1))</f>
-        <v>43504</v>
+        <v>43239</v>
       </c>
       <c r="D67" s="7">
         <f t="shared" ref="D67:D130" ca="1" si="5">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>98</v>
@@ -2839,17 +2836,17 @@
       <c r="A68" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C68" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43185</v>
+        <v>43271</v>
       </c>
       <c r="D68" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>99</v>
@@ -2862,13 +2859,13 @@
       <c r="A69" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="9" t="str">
+      <c r="B69" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>201</v>
       </c>
       <c r="C69" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43340</v>
+        <v>43520</v>
       </c>
       <c r="D69" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -2890,11 +2887,11 @@
       </c>
       <c r="B70" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C70" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43456</v>
+        <v>43257</v>
       </c>
       <c r="D70" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -2916,15 +2913,15 @@
       </c>
       <c r="B71" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C71" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43435</v>
+        <v>43413</v>
       </c>
       <c r="D71" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>102</v>
@@ -2942,15 +2939,15 @@
       </c>
       <c r="B72" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C72" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43406</v>
+        <v>43422</v>
       </c>
       <c r="D72" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>103</v>
@@ -2966,17 +2963,17 @@
       <c r="A73" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="9" t="str">
+      <c r="B73" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>203</v>
       </c>
       <c r="C73" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43372</v>
+        <v>43299</v>
       </c>
       <c r="D73" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>104</v>
@@ -2994,15 +2991,15 @@
       </c>
       <c r="B74" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="C74" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43108</v>
+        <v>43311</v>
       </c>
       <c r="D74" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>105</v>
@@ -3020,11 +3017,11 @@
       </c>
       <c r="B75" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="C75" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43437</v>
+        <v>43101</v>
       </c>
       <c r="D75" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3044,17 +3041,17 @@
       <c r="A76" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C76" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43155</v>
+        <v>43208</v>
       </c>
       <c r="D76" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>107</v>
@@ -3070,13 +3067,13 @@
       <c r="A77" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="9" t="str">
+      <c r="B77" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>207</v>
       </c>
       <c r="C77" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43281</v>
+        <v>43201</v>
       </c>
       <c r="D77" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3098,15 +3095,15 @@
       </c>
       <c r="B78" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C78" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43129</v>
+        <v>43385</v>
       </c>
       <c r="D78" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>109</v>
@@ -3124,15 +3121,15 @@
       </c>
       <c r="B79" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C79" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43323</v>
+        <v>43112</v>
       </c>
       <c r="D79" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>110</v>
@@ -3148,17 +3145,17 @@
       <c r="A80" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B80" s="9" t="str">
+      <c r="B80" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>241</v>
       </c>
       <c r="C80" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43198</v>
+        <v>43442</v>
       </c>
       <c r="D80" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>111</v>
@@ -3176,15 +3173,15 @@
       </c>
       <c r="B81" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C81" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43302</v>
+        <v>43215</v>
       </c>
       <c r="D81" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>112</v>
@@ -3199,15 +3196,15 @@
       </c>
       <c r="B82" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C82" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43323</v>
+        <v>43163</v>
       </c>
       <c r="D82" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>113</v>
@@ -3225,11 +3222,11 @@
       </c>
       <c r="B83" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C83" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43136</v>
+        <v>43347</v>
       </c>
       <c r="D83" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3251,15 +3248,15 @@
       </c>
       <c r="B84" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C84" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43144</v>
+        <v>43147</v>
       </c>
       <c r="D84" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>115</v>
@@ -3277,15 +3274,15 @@
       </c>
       <c r="B85" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C85" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43414</v>
+        <v>43201</v>
       </c>
       <c r="D85" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>116</v>
@@ -3303,15 +3300,15 @@
       </c>
       <c r="B86" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="C86" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43520</v>
+        <v>43319</v>
       </c>
       <c r="D86" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>117</v>
@@ -3329,15 +3326,15 @@
       </c>
       <c r="B87" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C87" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43334</v>
+        <v>43106</v>
       </c>
       <c r="D87" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>118</v>
@@ -3352,15 +3349,15 @@
       </c>
       <c r="B88" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C88" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43484</v>
+        <v>43132</v>
       </c>
       <c r="D88" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>119</v>
@@ -3378,15 +3375,15 @@
       </c>
       <c r="B89" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="C89" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43226</v>
+        <v>43200</v>
       </c>
       <c r="D89" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>120</v>
@@ -3399,13 +3396,13 @@
       <c r="A90" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B90" s="9" t="str">
+      <c r="B90" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>201</v>
       </c>
       <c r="C90" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43248</v>
+        <v>43245</v>
       </c>
       <c r="D90" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3424,15 +3421,15 @@
       </c>
       <c r="B91" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="C91" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43283</v>
+        <v>43333</v>
       </c>
       <c r="D91" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>122</v>
@@ -3448,13 +3445,13 @@
       <c r="A92" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="9" t="str">
+      <c r="B92" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>241</v>
       </c>
       <c r="C92" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43465</v>
+        <v>43449</v>
       </c>
       <c r="D92" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3480,11 +3477,11 @@
       </c>
       <c r="C93" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43219</v>
+        <v>43142</v>
       </c>
       <c r="D93" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>124</v>
@@ -3500,17 +3497,17 @@
       <c r="A94" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C94" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43367</v>
+        <v>43369</v>
       </c>
       <c r="D94" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>125</v>
@@ -3528,15 +3525,15 @@
       </c>
       <c r="B95" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="C95" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43377</v>
+        <v>43326</v>
       </c>
       <c r="D95" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>126</v>
@@ -3554,15 +3551,15 @@
       </c>
       <c r="B96" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="C96" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43498</v>
+        <v>43470</v>
       </c>
       <c r="D96" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>127</v>
@@ -3580,11 +3577,11 @@
       </c>
       <c r="B97" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="C97" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43509</v>
+        <v>43398</v>
       </c>
       <c r="D97" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3610,11 +3607,11 @@
       </c>
       <c r="C98" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43229</v>
+        <v>43409</v>
       </c>
       <c r="D98" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>129</v>
@@ -3632,15 +3629,15 @@
       </c>
       <c r="B99" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="C99" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43263</v>
+        <v>43391</v>
       </c>
       <c r="D99" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>130</v>
@@ -3662,11 +3659,11 @@
       </c>
       <c r="C100" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43268</v>
+        <v>43345</v>
       </c>
       <c r="D100" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>131</v>
@@ -3684,11 +3681,11 @@
       </c>
       <c r="B101" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="C101" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43168</v>
+        <v>43424</v>
       </c>
       <c r="D101" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3714,11 +3711,11 @@
       </c>
       <c r="C102" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43257</v>
+        <v>43193</v>
       </c>
       <c r="D102" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>133</v>
@@ -3736,15 +3733,15 @@
       </c>
       <c r="B103" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C103" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43217</v>
+        <v>43499</v>
       </c>
       <c r="D103" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>134</v>
@@ -3762,15 +3759,15 @@
       </c>
       <c r="B104" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="C104" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43275</v>
+        <v>43105</v>
       </c>
       <c r="D104" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>135</v>
@@ -3783,13 +3780,13 @@
       <c r="A105" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B105" s="9">
+      <c r="B105" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>W266</v>
       </c>
       <c r="C105" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43491</v>
+        <v>43211</v>
       </c>
       <c r="D105" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3808,11 +3805,11 @@
       </c>
       <c r="B106" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C106" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43190</v>
+        <v>43278</v>
       </c>
       <c r="D106" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3832,13 +3829,13 @@
       <c r="A107" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B107" s="9" t="str">
+      <c r="B107" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>W266</v>
+        <v>209</v>
       </c>
       <c r="C107" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43102</v>
+        <v>43193</v>
       </c>
       <c r="D107" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3857,11 +3854,11 @@
       </c>
       <c r="B108" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C108" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43475</v>
+        <v>43120</v>
       </c>
       <c r="D108" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -3883,15 +3880,15 @@
       </c>
       <c r="B109" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C109" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43480</v>
+        <v>43389</v>
       </c>
       <c r="D109" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>140</v>
@@ -3906,15 +3903,15 @@
       </c>
       <c r="B110" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="C110" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43313</v>
+        <v>43496</v>
       </c>
       <c r="D110" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>141</v>
@@ -3932,15 +3929,15 @@
       </c>
       <c r="B111" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="C111" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43276</v>
+        <v>43482</v>
       </c>
       <c r="D111" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>142</v>
@@ -3958,15 +3955,15 @@
       </c>
       <c r="B112" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>266</v>
+        <v>203</v>
       </c>
       <c r="C112" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43462</v>
+        <v>43233</v>
       </c>
       <c r="D112" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>143</v>
@@ -3981,15 +3978,15 @@
       </c>
       <c r="B113" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="C113" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43427</v>
+        <v>43489</v>
       </c>
       <c r="D113" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>144</v>
@@ -4007,15 +4004,15 @@
       </c>
       <c r="B114" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C114" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43502</v>
+        <v>43503</v>
       </c>
       <c r="D114" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>145</v>
@@ -4030,15 +4027,15 @@
       </c>
       <c r="B115" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C115" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43387</v>
+        <v>43503</v>
       </c>
       <c r="D115" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>146</v>
@@ -4054,17 +4051,17 @@
       <c r="A116" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B116" s="9">
+      <c r="B116" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>W266</v>
       </c>
       <c r="C116" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43187</v>
+        <v>43277</v>
       </c>
       <c r="D116" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>147</v>
@@ -4079,15 +4076,15 @@
       </c>
       <c r="B117" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C117" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43170</v>
+        <v>43214</v>
       </c>
       <c r="D117" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>148</v>
@@ -4102,11 +4099,11 @@
       </c>
       <c r="B118" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="C118" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43186</v>
+        <v>43226</v>
       </c>
       <c r="D118" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -4129,11 +4126,11 @@
       </c>
       <c r="C119" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43434</v>
+        <v>43277</v>
       </c>
       <c r="D119" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>150</v>
@@ -4152,11 +4149,11 @@
       </c>
       <c r="C120" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43325</v>
+        <v>43110</v>
       </c>
       <c r="D120" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>151</v>
@@ -4175,11 +4172,11 @@
       </c>
       <c r="C121" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43226</v>
+        <v>43399</v>
       </c>
       <c r="D121" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>152</v>
@@ -4194,11 +4191,11 @@
       </c>
       <c r="B122" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C122" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43286</v>
+        <v>43378</v>
       </c>
       <c r="D122" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -4218,13 +4215,13 @@
       <c r="A123" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B123" s="9">
+      <c r="B123" s="9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>209</v>
+        <v>W266</v>
       </c>
       <c r="C123" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43516</v>
+        <v>43129</v>
       </c>
       <c r="D123" s="7">
         <f t="shared" ca="1" si="5"/>
@@ -4246,15 +4243,15 @@
       </c>
       <c r="B124" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="C124" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43403</v>
+        <v>43427</v>
       </c>
       <c r="D124" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>154</v>
@@ -4269,15 +4266,15 @@
       </c>
       <c r="B125" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="C125" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43373</v>
+        <v>43487</v>
       </c>
       <c r="D125" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>155</v>
@@ -4293,63 +4290,63 @@
       <c r="A126" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B126" s="9">
+      <c r="B126" s="9" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>W266</v>
+      </c>
+      <c r="C126" s="6">
+        <f t="shared" ca="1" si="4"/>
+        <v>43434</v>
+      </c>
+      <c r="D126" s="7">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="12.75">
+      <c r="A127" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B127" s="9">
         <f t="shared" ca="1" si="3"/>
         <v>200</v>
       </c>
-      <c r="C126" s="6">
+      <c r="C127" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43513</v>
-      </c>
-      <c r="D126" s="7">
+        <v>43228</v>
+      </c>
+      <c r="D127" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F126" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F127" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="12.75">
-      <c r="A127" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B127" s="9">
+    <row r="128" spans="1:7" ht="12.75">
+      <c r="A128" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B128" s="9">
         <f t="shared" ca="1" si="3"/>
         <v>266</v>
       </c>
-      <c r="C127" s="6">
+      <c r="C128" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43323</v>
-      </c>
-      <c r="D127" s="7">
+        <v>43293</v>
+      </c>
+      <c r="D128" s="7">
         <f t="shared" ca="1" si="5"/>
         <v>1</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" ht="12.75">
-      <c r="A128" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B128" s="9">
-        <f t="shared" ca="1" si="3"/>
-        <v>241</v>
-      </c>
-      <c r="C128" s="6">
-        <f t="shared" ca="1" si="4"/>
-        <v>43453</v>
-      </c>
-      <c r="D128" s="7">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>158</v>
@@ -4368,11 +4365,11 @@
       </c>
       <c r="C129" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43262</v>
+        <v>43377</v>
       </c>
       <c r="D129" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>159</v>
@@ -4390,15 +4387,15 @@
       </c>
       <c r="B130" s="9">
         <f t="shared" ref="B130:B193" ca="1" si="6">CHOOSE(RANDBETWEEN(1,10), 200,201,203,207,209,210,241,231,266, "W266")</f>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C130" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>43148</v>
+        <v>43231</v>
       </c>
       <c r="D130" s="7">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>160</v>
@@ -4416,15 +4413,15 @@
       </c>
       <c r="B131" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C131" s="6">
         <f t="shared" ref="C131:C194" ca="1" si="7">RANDBETWEEN(DATE(2018,1,1),DATE(2019,3,1))</f>
-        <v>43400</v>
+        <v>43214</v>
       </c>
       <c r="D131" s="7">
         <f t="shared" ref="D131:D194" ca="1" si="8">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>161</v>
@@ -4446,7 +4443,7 @@
       </c>
       <c r="C132" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43293</v>
+        <v>43315</v>
       </c>
       <c r="D132" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4468,15 +4465,15 @@
       </c>
       <c r="B133" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C133" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43305</v>
+        <v>43201</v>
       </c>
       <c r="D133" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>163</v>
@@ -4495,11 +4492,11 @@
       </c>
       <c r="C134" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43145</v>
+        <v>43121</v>
       </c>
       <c r="D134" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>164</v>
@@ -4512,13 +4509,13 @@
       <c r="A135" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B135" s="9">
+      <c r="B135" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>W266</v>
       </c>
       <c r="C135" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43296</v>
+        <v>43501</v>
       </c>
       <c r="D135" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4537,15 +4534,15 @@
       </c>
       <c r="B136" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C136" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43455</v>
+        <v>43482</v>
       </c>
       <c r="D136" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>166</v>
@@ -4567,11 +4564,11 @@
       </c>
       <c r="C137" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43222</v>
+        <v>43434</v>
       </c>
       <c r="D137" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>167</v>
@@ -4586,11 +4583,11 @@
       </c>
       <c r="B138" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C138" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43269</v>
+        <v>43421</v>
       </c>
       <c r="D138" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4609,15 +4606,15 @@
       </c>
       <c r="B139" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="C139" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43343</v>
+        <v>43265</v>
       </c>
       <c r="D139" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>169</v>
@@ -4632,15 +4629,15 @@
       </c>
       <c r="B140" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C140" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43476</v>
+        <v>43336</v>
       </c>
       <c r="D140" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>170</v>
@@ -4653,13 +4650,13 @@
       <c r="A141" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B141" s="9" t="str">
+      <c r="B141" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>W266</v>
+        <v>209</v>
       </c>
       <c r="C141" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43335</v>
+        <v>43498</v>
       </c>
       <c r="D141" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4678,15 +4675,15 @@
       </c>
       <c r="B142" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="C142" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43224</v>
+        <v>43205</v>
       </c>
       <c r="D142" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E142" s="4" t="s">
         <v>172</v>
@@ -4701,15 +4698,15 @@
       </c>
       <c r="B143" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C143" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43424</v>
+        <v>43283</v>
       </c>
       <c r="D143" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>174</v>
@@ -4725,17 +4722,17 @@
       <c r="A144" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B144" s="9">
+      <c r="B144" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>231</v>
+        <v>W266</v>
       </c>
       <c r="C144" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43396</v>
+        <v>43518</v>
       </c>
       <c r="D144" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>175</v>
@@ -4754,7 +4751,7 @@
       </c>
       <c r="C145" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43355</v>
+        <v>43295</v>
       </c>
       <c r="D145" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4773,11 +4770,11 @@
       </c>
       <c r="B146" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C146" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43129</v>
+        <v>43425</v>
       </c>
       <c r="D146" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -4799,15 +4796,15 @@
       </c>
       <c r="B147" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C147" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43331</v>
+        <v>43458</v>
       </c>
       <c r="D147" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>178</v>
@@ -4826,11 +4823,11 @@
       </c>
       <c r="C148" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43469</v>
+        <v>43518</v>
       </c>
       <c r="D148" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>179</v>
@@ -4846,17 +4843,17 @@
       <c r="A149" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B149" s="9">
+      <c r="B149" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>W266</v>
       </c>
       <c r="C149" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43167</v>
+        <v>43454</v>
       </c>
       <c r="D149" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E149" s="4" t="s">
         <v>180</v>
@@ -4869,17 +4866,17 @@
       <c r="A150" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B150" s="9">
+      <c r="B150" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>210</v>
+        <v>W266</v>
       </c>
       <c r="C150" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43321</v>
+        <v>43339</v>
       </c>
       <c r="D150" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>181</v>
@@ -4895,17 +4892,17 @@
       <c r="A151" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B151" s="9" t="str">
+      <c r="B151" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>W266</v>
+        <v>266</v>
       </c>
       <c r="C151" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43459</v>
+        <v>43266</v>
       </c>
       <c r="D151" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>182</v>
@@ -4923,15 +4920,15 @@
       </c>
       <c r="B152" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C152" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43305</v>
+        <v>43261</v>
       </c>
       <c r="D152" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>183</v>
@@ -4949,15 +4946,15 @@
       </c>
       <c r="B153" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C153" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43417</v>
+        <v>43411</v>
       </c>
       <c r="D153" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>184</v>
@@ -4975,15 +4972,15 @@
       </c>
       <c r="B154" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C154" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43437</v>
+        <v>43280</v>
       </c>
       <c r="D154" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>185</v>
@@ -5001,15 +4998,15 @@
       </c>
       <c r="B155" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C155" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43367</v>
+        <v>43180</v>
       </c>
       <c r="D155" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>186</v>
@@ -5031,7 +5028,7 @@
       </c>
       <c r="C156" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43239</v>
+        <v>43166</v>
       </c>
       <c r="D156" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -5051,17 +5048,17 @@
       <c r="A157" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B157" s="9">
+      <c r="B157" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>W266</v>
       </c>
       <c r="C157" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43509</v>
+        <v>43363</v>
       </c>
       <c r="D157" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E157" s="4" t="s">
         <v>188</v>
@@ -5076,15 +5073,15 @@
       </c>
       <c r="B158" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C158" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43151</v>
+        <v>43363</v>
       </c>
       <c r="D158" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E158" s="4" t="s">
         <v>189</v>
@@ -5102,15 +5099,15 @@
       </c>
       <c r="B159" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="C159" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43123</v>
+        <v>43160</v>
       </c>
       <c r="D159" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>83</v>
@@ -5121,9 +5118,7 @@
       <c r="G159" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H159" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="H159" s="2"/>
     </row>
     <row r="160" spans="1:8" ht="12.75">
       <c r="A160" s="4" t="s">
@@ -5131,51 +5126,47 @@
       </c>
       <c r="B160" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>209</v>
       </c>
       <c r="C160" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43494</v>
+        <v>43346</v>
       </c>
       <c r="D160" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H160" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="H160" s="2"/>
     </row>
     <row r="161" spans="1:8" ht="12.75">
       <c r="A161" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B161" s="9">
+      <c r="B161" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>W266</v>
       </c>
       <c r="C161" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43287</v>
+        <v>43114</v>
       </c>
       <c r="D161" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H161" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="H161" s="2"/>
     </row>
     <row r="162" spans="1:8" ht="25.5">
       <c r="A162" s="4" t="s">
@@ -5183,11 +5174,11 @@
       </c>
       <c r="B162" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C162" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43184</v>
+        <v>43250</v>
       </c>
       <c r="D162" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -5202,9 +5193,7 @@
       <c r="G162" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H162" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="H162" s="2"/>
     </row>
     <row r="163" spans="1:8" ht="25.5">
       <c r="A163" s="4" t="s">
@@ -5212,25 +5201,23 @@
       </c>
       <c r="B163" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C163" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43243</v>
+        <v>43130</v>
       </c>
       <c r="D163" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H163" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="H163" s="2"/>
     </row>
     <row r="164" spans="1:8" ht="12.75">
       <c r="A164" s="4" t="s">
@@ -5238,18 +5225,18 @@
       </c>
       <c r="B164" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C164" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43349</v>
+        <v>43365</v>
       </c>
       <c r="D164" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>42</v>
@@ -5261,18 +5248,18 @@
       </c>
       <c r="B165" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C165" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43236</v>
+        <v>43187</v>
       </c>
       <c r="D165" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>8</v>
@@ -5287,18 +5274,18 @@
       </c>
       <c r="B166" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C166" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43358</v>
+        <v>43407</v>
       </c>
       <c r="D166" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>8</v>
@@ -5313,18 +5300,18 @@
       </c>
       <c r="B167" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C167" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43468</v>
+        <v>43491</v>
       </c>
       <c r="D167" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>4</v>
@@ -5334,20 +5321,20 @@
       <c r="A168" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B168" s="9">
+      <c r="B168" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>W266</v>
       </c>
       <c r="C168" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43416</v>
+        <v>43219</v>
       </c>
       <c r="D168" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>29</v>
@@ -5359,18 +5346,18 @@
       </c>
       <c r="B169" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="C169" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43219</v>
+        <v>43103</v>
       </c>
       <c r="D169" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>29</v>
@@ -5380,20 +5367,20 @@
       <c r="A170" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B170" s="9" t="str">
+      <c r="B170" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>W266</v>
+        <v>203</v>
       </c>
       <c r="C170" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43292</v>
+        <v>43120</v>
       </c>
       <c r="D170" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>42</v>
@@ -5412,14 +5399,14 @@
       </c>
       <c r="C171" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43336</v>
+        <v>43169</v>
       </c>
       <c r="D171" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>4</v>
@@ -5434,18 +5421,18 @@
       </c>
       <c r="B172" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>203</v>
       </c>
       <c r="C172" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43161</v>
+        <v>43192</v>
       </c>
       <c r="D172" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>29</v>
@@ -5457,18 +5444,18 @@
       </c>
       <c r="B173" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="C173" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43320</v>
+        <v>43515</v>
       </c>
       <c r="D173" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>29</v>
@@ -5480,18 +5467,18 @@
       </c>
       <c r="B174" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C174" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43173</v>
+        <v>43405</v>
       </c>
       <c r="D174" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>29</v>
@@ -5503,18 +5490,18 @@
       </c>
       <c r="B175" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="C175" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43210</v>
+        <v>43501</v>
       </c>
       <c r="D175" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>29</v>
@@ -5530,14 +5517,14 @@
       </c>
       <c r="C176" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43249</v>
+        <v>43394</v>
       </c>
       <c r="D176" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>4</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>29</v>
@@ -5549,18 +5536,18 @@
       </c>
       <c r="B177" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C177" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43106</v>
+        <v>43402</v>
       </c>
       <c r="D177" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>29</v>
@@ -5576,14 +5563,14 @@
       </c>
       <c r="C178" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43409</v>
+        <v>43224</v>
       </c>
       <c r="D178" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>17</v>
@@ -5598,18 +5585,18 @@
       </c>
       <c r="B179" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C179" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43355</v>
+        <v>43464</v>
       </c>
       <c r="D179" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>29</v>
@@ -5621,18 +5608,18 @@
       </c>
       <c r="B180" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="C180" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43480</v>
+        <v>43278</v>
       </c>
       <c r="D180" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>29</v>
@@ -5644,18 +5631,18 @@
       </c>
       <c r="B181" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C181" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43367</v>
+        <v>43207</v>
       </c>
       <c r="D181" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>4</v>
       </c>
       <c r="E181" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>23</v>
@@ -5667,18 +5654,18 @@
       </c>
       <c r="B182" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="C182" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43482</v>
+        <v>43158</v>
       </c>
       <c r="D182" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E182" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>29</v>
@@ -5690,18 +5677,18 @@
       </c>
       <c r="B183" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C183" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43457</v>
+        <v>43381</v>
       </c>
       <c r="D183" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>1</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>8</v>
@@ -5714,20 +5701,20 @@
       <c r="A184" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B184" s="9">
+      <c r="B184" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>W266</v>
       </c>
       <c r="C184" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43144</v>
+        <v>43481</v>
       </c>
       <c r="D184" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>4</v>
@@ -5742,18 +5729,18 @@
       </c>
       <c r="B185" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="C185" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43333</v>
+        <v>43473</v>
       </c>
       <c r="D185" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>4</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>23</v>
@@ -5765,18 +5752,18 @@
       </c>
       <c r="B186" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="C186" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43357</v>
+        <v>43333</v>
       </c>
       <c r="D186" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F186" s="2" t="s">
         <v>29</v>
@@ -5788,18 +5775,18 @@
       </c>
       <c r="B187" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C187" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43123</v>
+        <v>43525</v>
       </c>
       <c r="D187" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>2</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>17</v>
@@ -5814,18 +5801,18 @@
       </c>
       <c r="B188" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="C188" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43431</v>
+        <v>43468</v>
       </c>
       <c r="D188" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F188" s="2" t="s">
         <v>17</v>
@@ -5840,18 +5827,18 @@
       </c>
       <c r="B189" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="C189" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43468</v>
+        <v>43179</v>
       </c>
       <c r="D189" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F189" s="2" t="s">
         <v>29</v>
@@ -5861,20 +5848,20 @@
       <c r="A190" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B190" s="9">
+      <c r="B190" s="9" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>209</v>
+        <v>W266</v>
       </c>
       <c r="C190" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43255</v>
+        <v>43231</v>
       </c>
       <c r="D190" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>2</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>17</v>
@@ -5889,18 +5876,18 @@
       </c>
       <c r="B191" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>209</v>
       </c>
       <c r="C191" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43424</v>
+        <v>43199</v>
       </c>
       <c r="D191" s="7">
         <f t="shared" ca="1" si="8"/>
         <v>5</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F191" s="2" t="s">
         <v>29</v>
@@ -5912,18 +5899,18 @@
       </c>
       <c r="B192" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C192" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43267</v>
+        <v>43112</v>
       </c>
       <c r="D192" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F192" s="2" t="s">
         <v>17</v>
@@ -5938,18 +5925,18 @@
       </c>
       <c r="B193" s="9">
         <f t="shared" ca="1" si="6"/>
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="C193" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43502</v>
+        <v>43160</v>
       </c>
       <c r="D193" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F193" s="2" t="s">
         <v>8</v>
@@ -5964,18 +5951,18 @@
       </c>
       <c r="B194" s="9">
         <f ca="1">CHOOSE(RANDBETWEEN(1,10), 200,201,203,207,209,210,241,231,266, "W266")</f>
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="C194" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>43258</v>
+        <v>43323</v>
       </c>
       <c r="D194" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F194" s="2" t="s">
         <v>34</v>

</xml_diff>